<commit_message>
update template to version 4 (xlsx and csv); add WHO field mappings to xlsx, update README
</commit_message>
<xml_diff>
--- a/PHA4GE to Sequence Repository Field Mappings.xlsx
+++ b/PHA4GE to Sequence Repository Field Mappings.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fda-my.sharepoint.com/personal/ruth_timme_fda_gov/Documents/workingGroups-Projects/PHA4GE/SARS-CoV-2 metadata spec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inesmendes/Documents/PHA4GE/SARS-CoV-2-Contextual-Data-Specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{51042134-DAB5-D344-9564-0FBD49DC2C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E146FC95-68C3-504E-9B7D-6922032300AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8C2D17-B355-E34D-8B90-EB55AED2CBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23900" windowHeight="25860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23900" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GISAID to PHA4GE field mappings" sheetId="3" r:id="rId1"/>
     <sheet name="ENA to PHA4GE field mappings" sheetId="4" r:id="rId2"/>
     <sheet name="NCBI to PHA4GE field mappings" sheetId="5" r:id="rId3"/>
+    <sheet name="WHO to PHA4GE field mappings" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'NCBI to PHA4GE field mappings'!$A$4:$F$39</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="632">
   <si>
     <t>bioproject accession</t>
   </si>
@@ -1731,6 +1732,280 @@
   <si>
     <t>additional wastewater attributes being developed</t>
   </si>
+  <si>
+    <t>WHO Metadata Type</t>
+  </si>
+  <si>
+    <t>Field Label</t>
+  </si>
+  <si>
+    <t>WHO Details</t>
+  </si>
+  <si>
+    <t>Core Metadata</t>
+  </si>
+  <si>
+    <t>Sample Identification number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field can be populated by the PHA4GE field "specimen collector sample ID". </t>
+  </si>
+  <si>
+    <t>Sample type</t>
+  </si>
+  <si>
+    <t>Examples: "sputum", "blood", "serum", "saliva", "stool", "nasopharyngeal swab", "wastewater"</t>
+  </si>
+  <si>
+    <t>anatomical material, anatomical part, body product, environmental material, environmental site, collection device, collection method</t>
+  </si>
+  <si>
+    <t>The WHO field can be populated by concatenating the information included in the PHA4GE fields "anatomical material", "anatomical part", "body product", "environmental material", "environmental site", "collection device", and "collection method", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>Sample collection date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field can be populated by the PHA4GE field "sample collection date". </t>
+  </si>
+  <si>
+    <t>Country of collection</t>
+  </si>
+  <si>
+    <t>geo_loc name (country)</t>
+  </si>
+  <si>
+    <t>State/province of collection</t>
+  </si>
+  <si>
+    <t>geo_loc name (state/province/territory)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field can be populated by the PHA4GE field "geo_loc name (state/province/territory)". </t>
+  </si>
+  <si>
+    <t>Originating diagnostic lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field can be populated by the PHA4GE field "sample collected by". </t>
+  </si>
+  <si>
+    <t>Sequence submitting lab</t>
+  </si>
+  <si>
+    <t>Where sequence data have been generated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field can be populated by the PHA4GE field "sequence submitted by". </t>
+  </si>
+  <si>
+    <t>Sampling method</t>
+  </si>
+  <si>
+    <t>Part of routine surveillance or focused sampling, representative or targeted sampling</t>
+  </si>
+  <si>
+    <t>PHA4GE distinguishes between the criteria for sampling encoded by "purpose of sampling" (i.e. why a sample was collected) and the criteria for sequencing (i.e. why certain samples were selected for sequencing e.g. baseline surveilance (random sampling), targeted surveillance, outbreak/cluster investigation, research etc). The sampling strategy is addressed by four different fields in the PHA4GE specification. The WHO field can be populated by the PHA4GE "purpose of sequencing" field, but additional information can be found in the PHA4GE fields "purpose of sampling", as well as "purpose of sequeincg details" and "purpose of sampling details".</t>
+  </si>
+  <si>
+    <t>e.g. human, animal (specifics), environment, unknown</t>
+  </si>
+  <si>
+    <t>The PHA4GE specification distinguishes host names as either common name and scientific name. The WHO field should be populated by the PHA4GE field "host (scientific name)".</t>
+  </si>
+  <si>
+    <t>Descriptive Metadata</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>PHA4GE also has “host age unit” and “host age bin”</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>e.g. male, female, other, unknown</t>
+  </si>
+  <si>
+    <t>While not an exact semantic match, the WHO field can be populated by the PHA4GE field "host gender".</t>
+  </si>
+  <si>
+    <t>Race and/or ethnicity</t>
+  </si>
+  <si>
+    <t>host ethnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This field can be populated by the PHA4GE field "host ethnicity". </t>
+  </si>
+  <si>
+    <t>Health worker status</t>
+  </si>
+  <si>
+    <t>e.g. yes, no, unknown. See HW definition in surveillance protocol for Health Workers</t>
+  </si>
+  <si>
+    <t>host role</t>
+  </si>
+  <si>
+    <t>The PHA4GE field “host role” contains many professional descriptors. If a descriptor matching a WHO prescribed Health Worker is appropriate, populate the WHO field with "yes". If a descriptor is provided that does not match a WHO prescribed Health Worker, put "no". If no information is provided, or the information is not clear, put "unknown".</t>
+  </si>
+  <si>
+    <t>Travel History</t>
+  </si>
+  <si>
+    <t>Location(s) and timing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">travel history, destination of most recent travel (city), destination of most recent travel (state/province/territory), destination of most recent travel (country), most recent travel departure date, most recent travel return date
+, 
+</t>
+  </si>
+  <si>
+    <t>PHA4GE has several fields to capture information about recent travel. The WHO field can be populated by concatenating information from the PHA4GE fields "travel history" (i.e. travel in the last 6 months), "destination of most recent travel (city)", "destination of most recent travel (state/province/territory)", "destination of most recent travel (country)", "most recent travel departure date", and "most recent travel return date", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>Metadata for Characterization</t>
+  </si>
+  <si>
+    <t>RT-PCR assay used (if any)</t>
+  </si>
+  <si>
+    <t>This field can be populated by the PHA4GE field "diagnostic pcr protocol 1". If more than one gene was tested in subsequent/multiplex assays, concatenate information from "diagnostic pcr protocol 2", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>RT-PCR Ct value (if any)</t>
+  </si>
+  <si>
+    <t>This field can be populated by the PHA4GE field "diagnostic pcr Ct value 1". If more than one gene was tested in subsequent/multiplex assays, concatenate information from "diagnostic pcr Ct value 2", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>Symptomatic</t>
+  </si>
+  <si>
+    <t>e.g. yes, no, unknown.</t>
+  </si>
+  <si>
+    <t>PHA4GE specifies whether an individual is symptomatic as a value under the "host health state" field. Populate the WHO field with "yes" when a PHA4GE "Symptomatic" tag is present under "host health state". Put "no" is a PHA4GE "Asymptmmatic" tage is present. Put "unknown" if no tags specifying symptomatic state are present.</t>
+  </si>
+  <si>
+    <t>Vaccination status (for humans)</t>
+  </si>
+  <si>
+    <t>Date of vaccination (dose 1 and/or dose 2, as needed), vaccine type, source of information (documented evidence such as vaccine register or vaccine card versus recall)</t>
+  </si>
+  <si>
+    <t>host vaccination status, vaccine name, number of vaccine doses received, first dose vaccination date, last dose vaccination date</t>
+  </si>
+  <si>
+    <t>PHA4GE has several fields to describe the vaccine types and doses administered. Populate the WHO field by concatenating information from "host vaccination status", "vaccine name, number of vaccine doses received" (make sure to add the words "doses received" after the number), "first dose vaccination date", and "last dose vaccination date", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>Date of symptom onset</t>
+  </si>
+  <si>
+    <t>symptom onset date</t>
+  </si>
+  <si>
+    <t>This field can be populated by the PHA4GE field "symptom onset date".</t>
+  </si>
+  <si>
+    <t>Hospitalization status</t>
+  </si>
+  <si>
+    <t>e.g. ever hospitalized, never hospitalized, unknown</t>
+  </si>
+  <si>
+    <t>Hospitalized</t>
+  </si>
+  <si>
+    <t>PHA4GE specifies whether an individual was hospitalized as a value under the "host health status details" field. Populate the WHO field with "yes" when a PHA4GE "Hospitalized" tag is present under "host health status details". Put "no" if it is known that the individual was not hospitalized (i.e. if they are asymptomatic). Put "unknown" if no tags specifying hospitalization state are present.</t>
+  </si>
+  <si>
+    <t>Admission to intensive care unit (ICU)</t>
+  </si>
+  <si>
+    <t>e.g. yes, no, unknown</t>
+  </si>
+  <si>
+    <t>Hospitalized (ICU)</t>
+  </si>
+  <si>
+    <t>PHA4GE specifies whether an individual was hospitalized in the intensive care unit (ICU) as a value under the "host health status details" field. Populate the WHO field with "yes" when a PHA4GE "Hospitalized (ICU)" tag is present under "host health status details". Put "no" if it is known that the individual was not hospitalized (i.e. if they are asymptomatic) or it is known that the individual was hospitalized but not in the ICU. Put "unknown" if no tags specifying hospitalization state are present.</t>
+  </si>
+  <si>
+    <t>Mechanical ventilation</t>
+  </si>
+  <si>
+    <t>PHA4GE specifies whether an individual was mechanically ventilated as a value under the "host health status details" field. Populate the WHO field with "yes" when a PHA4GE "Mechanical ventilation" tag is present under "host health status details". Put "no" if it is known that the individual was not mechanically ventilated  or it is known that the individual was hospitalized (i.e. if they are asymptomatic). Put "unknown" if no tags specifying hospitalization state are present.</t>
+  </si>
+  <si>
+    <t>Outcome</t>
+  </si>
+  <si>
+    <t>Deceased/recovered</t>
+  </si>
+  <si>
+    <t>This field can be populated by the PHA4GE field "host disease outcome".</t>
+  </si>
+  <si>
+    <t>Past history of SARS-CoV-2 infection and date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prior SARS-CoV-2 infection, prior SARS-CoV-2 infection isolate, prior SARS-CoV-2 infection date
+</t>
+  </si>
+  <si>
+    <t>PHA4GE has several fields to capture information about prior SARS-CoV-2 infections date. Populate the WHO field by concatenating information from the PHA4GE fields "prior SARS-CoV-2 infection", "prior SARS-CoV-2 infection isolate", and "prior SARS-CoV-2 infection date", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>Therapeutics received</t>
+  </si>
+  <si>
+    <t>COVID-19-specific</t>
+  </si>
+  <si>
+    <t>prior SARS-CoV-2 antiviral treatment, prior SARS-CoV-2 antiviral treatment agent, prior SARS-CoV-2 antiviral treatment date</t>
+  </si>
+  <si>
+    <t>PHA4GE has several fields to capture information about prior SARS-CoV-2 treatment. Populate the WHO field by concatenating information from the PHA4GE fields "prior SARS-CoV-2 antiviral treatment", "prior SARS-CoV-2 antiviral treatment agent", and "prior SARS-CoV-2 antiviral treatment date", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>Location of exposure, link to known cluster/ outbreak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location of exposure geo_loc name (country), exposure setting, exposure event, exposure details
+</t>
+  </si>
+  <si>
+    <t>PHA4GE has several fields to capture information about exposure details. Populate the WHO field by concatenating information from the PHA4GE fields "location of exposure geo_loc name (country)", "exposure setting", "exposure event", and "exposure details", separated by semicolons.</t>
+  </si>
+  <si>
+    <t>Contact with known animal reservoir</t>
+  </si>
+  <si>
+    <t>e.g. yes, no, unknown; and type(s) of animal(s)</t>
+  </si>
+  <si>
+    <t>No exact match</t>
+  </si>
+  <si>
+    <t>PHA4GE provides various animal-related pick list terms in different exposure fields that could apply e.g. Veterinarian, abattoir, farm etc. If an animal-related tag is present, populate the WHO field with this information.</t>
+  </si>
+  <si>
+    <t>Comorbidities</t>
+  </si>
+  <si>
+    <t>List comorbidities known to increase COVID-19 severity</t>
+  </si>
+  <si>
+    <t>pre-existing conditions and risk factors</t>
+  </si>
+  <si>
+    <t>This field can be populated by the PHA4GE field "pre-existing conditions and risk factors".</t>
+  </si>
 </sst>
 </file>
 
@@ -1867,7 +2142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1886,11 +2161,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2028,6 +2327,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60992,7 +61300,7 @@
   </sheetPr>
   <dimension ref="A1:AB1036"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -65578,4 +65886,497 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B78A16-33A2-0347-91B5-D787CF857889}">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="40.1640625" customWidth="1"/>
+    <col min="5" max="5" width="58.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="65" t="s">
+        <v>542</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>543</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>544</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A2" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>546</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+      <c r="A3" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>548</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>550</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B4" s="63" t="s">
+        <v>552</v>
+      </c>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A5" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>554</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A6" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>556</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69" t="s">
+        <v>557</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A7" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B7" s="63" t="s">
+        <v>559</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A8" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B8" s="63" t="s">
+        <v>561</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="154" x14ac:dyDescent="0.15">
+      <c r="A9" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B9" s="63" t="s">
+        <v>564</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>349</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.15">
+      <c r="A10" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="B10" s="63" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="68" t="s">
+        <v>569</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>570</v>
+      </c>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A12" s="68" t="s">
+        <v>569</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>572</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>573</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A13" s="68" t="s">
+        <v>569</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>575</v>
+      </c>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69" t="s">
+        <v>576</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+      <c r="A14" s="68" t="s">
+        <v>569</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>578</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>579</v>
+      </c>
+      <c r="D14" s="69" t="s">
+        <v>580</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="112" x14ac:dyDescent="0.15">
+      <c r="A15" s="68" t="s">
+        <v>569</v>
+      </c>
+      <c r="B15" s="63" t="s">
+        <v>582</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A16" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>587</v>
+      </c>
+      <c r="C16" s="69"/>
+      <c r="D16" s="11" t="s">
+        <v>413</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A17" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>589</v>
+      </c>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69" t="s">
+        <v>414</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+      <c r="A18" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>591</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>592</v>
+      </c>
+      <c r="D18" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+      <c r="A19" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B19" s="63" t="s">
+        <v>594</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A20" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>598</v>
+      </c>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69" t="s">
+        <v>599</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="98" x14ac:dyDescent="0.15">
+      <c r="A21" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B21" s="63" t="s">
+        <v>601</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="D21" s="69" t="s">
+        <v>603</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="112" x14ac:dyDescent="0.15">
+      <c r="A22" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>605</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="D22" s="69" t="s">
+        <v>607</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="112" x14ac:dyDescent="0.15">
+      <c r="A23" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>609</v>
+      </c>
+      <c r="C23" s="69" t="s">
+        <v>606</v>
+      </c>
+      <c r="D23" s="69" t="s">
+        <v>609</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A24" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>611</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="D24" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+      <c r="A25" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>614</v>
+      </c>
+      <c r="C25" s="69"/>
+      <c r="D25" s="11" t="s">
+        <v>615</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+      <c r="A26" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>617</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>618</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>619</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+      <c r="A27" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B27" s="63" t="s">
+        <v>621</v>
+      </c>
+      <c r="C27" s="69"/>
+      <c r="D27" s="11" t="s">
+        <v>622</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="56" x14ac:dyDescent="0.15">
+      <c r="A28" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>624</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>625</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.15">
+      <c r="A29" s="68" t="s">
+        <v>586</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>628</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>629</v>
+      </c>
+      <c r="D29" s="69" t="s">
+        <v>630</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>631</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>